<commit_message>
Add image of initial dev diagram and changes to docs.
</commit_message>
<xml_diff>
--- a/docs/AWS_SQL_Server_Container_Hosting_Strategy_diagram.xlsx
+++ b/docs/AWS_SQL_Server_Container_Hosting_Strategy_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1295cc705891211/Work/ProgrammingExperiments/ASP.NET/Pitcher/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67DEDEE9-CCF0-43DF-9810-0A925999DD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{67DEDEE9-CCF0-43DF-9810-0A925999DD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC940496-4976-425B-BA2A-DF753498E537}"/>
   <bookViews>
-    <workbookView xWindow="-5985" yWindow="18345" windowWidth="21600" windowHeight="11385" xr2:uid="{80A68369-CECB-4987-BA8A-C95284560FC2}"/>
+    <workbookView xWindow="13965" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{80A68369-CECB-4987-BA8A-C95284560FC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">            1. Push image</t>
+    <t xml:space="preserve">1. Push development </t>
+  </si>
+  <si>
+    <t xml:space="preserve">image. </t>
   </si>
 </sst>
 </file>
@@ -257,14 +260,14 @@
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -307,14 +310,14 @@
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -422,14 +425,14 @@
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="dk1"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -470,6 +473,62 @@
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38208</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC0480B3-208C-1BAC-E5E3-F23283C5CAE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="0"/>
+          <a:endCxn id="29" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3695808" y="3752850"/>
+          <a:ext cx="9418" cy="2762251"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -488,37 +547,180 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38208</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190606</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133420</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2007DA2E-73A9-B73F-955F-C0901CFA94AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="2105025"/>
+          <a:ext cx="762106" cy="504895"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>56857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38316</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>47626</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8B3A047-3FA5-2FB0-C229-D8AB0DC0FD0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect b="46271"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3086099" y="2723857"/>
+          <a:ext cx="1219417" cy="1028993"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>493212</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>35966</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{135CCFF8-9D37-EC3A-8EF3-2EA0596DA482}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791200" y="2647998"/>
+          <a:ext cx="1407612" cy="1197968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38316</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190354</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>8482</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC0480B3-208C-1BAC-E5E3-F23283C5CAE3}"/>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89522EAD-E603-4406-95B5-B7DF049706FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="0"/>
-          <a:endCxn id="29" idx="2"/>
+          <a:stCxn id="29" idx="3"/>
+          <a:endCxn id="31" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3695808" y="3752850"/>
-          <a:ext cx="9418" cy="2762251"/>
+        <a:xfrm>
+          <a:off x="4305516" y="3238354"/>
+          <a:ext cx="1485684" cy="8628"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -546,34 +748,106 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18982F68-72FE-AA7F-4D62-3034CFABEC0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4295776" y="2857500"/>
+          <a:ext cx="1581150" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Deploy </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>container to ECS </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>35966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>399006</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DCB06AB-9863-45A1-8E7E-89CB9D1C3216}"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74CA9545-EC86-478A-9C75-1897745E93FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="0"/>
+          <a:stCxn id="31" idx="2"/>
+          <a:endCxn id="3" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="7200900" y="5219700"/>
-          <a:ext cx="19051" cy="1314450"/>
+        <a:xfrm flipH="1">
+          <a:off x="4314826" y="3845966"/>
+          <a:ext cx="2180180" cy="2973935"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -599,180 +873,37 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190606</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>133420</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2007DA2E-73A9-B73F-955F-C0901CFA94AE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4914900" y="2105025"/>
-          <a:ext cx="762106" cy="504895"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>56857</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38316</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Picture 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8B3A047-3FA5-2FB0-C229-D8AB0DC0FD0F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect b="46271"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3086099" y="2723857"/>
-          <a:ext cx="1219417" cy="1028993"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171498</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>493212</xdr:colOff>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>399006</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>35966</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{135CCFF8-9D37-EC3A-8EF3-2EA0596DA482}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5791200" y="2647998"/>
-          <a:ext cx="1407612" cy="1197968"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38316</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>190354</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>8482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514351</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89522EAD-E603-4406-95B5-B7DF049706FB}"/>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53E13DF2-BEDE-451D-A1DC-EE32F04C8124}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="29" idx="3"/>
-          <a:endCxn id="31" idx="1"/>
+          <a:stCxn id="31" idx="2"/>
+          <a:endCxn id="9" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4305516" y="3238354"/>
-          <a:ext cx="1485684" cy="8628"/>
+          <a:off x="6495006" y="3845966"/>
+          <a:ext cx="724945" cy="2688184"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -798,7 +929,171 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>93270</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>65725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>595966</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>164104</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2923D3D4-CDBA-47BD-B065-836ED5D888F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18407000">
+          <a:off x="4086378" y="5673817"/>
+          <a:ext cx="1050879" cy="502696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Pull and run from</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> ECS </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>364604</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>185552</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>213209</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>12472</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6FBE37-CB64-4D23-97E0-D474B8C6CF39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="4523862">
+          <a:off x="6719097" y="5489659"/>
+          <a:ext cx="1160420" cy="458205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Pull and run from</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> ECS </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1098,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92BC4DF-A387-41E4-AAE5-CDB1A0FF6843}">
-  <dimension ref="E30"/>
+  <dimension ref="E30:E31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,6 +1409,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>